<commit_message>
LLM analyse en classification eval
</commit_message>
<xml_diff>
--- a/out/Title_Lead_Body.xlsx
+++ b/out/Title_Lead_Body.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semde\Documents\RWD_Sentiment_Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semde\Documents\RWD_Sentiment_Analyse\out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F24AA7B-02CE-4E3B-83D6-D868BBE3E22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A46AB6-FBA2-4369-B236-46A0565B8980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14595" xr2:uid="{B9B08F07-4D74-46C4-A83D-5267EA35051F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="227">
   <si>
     <t>id</t>
   </si>
@@ -957,9 +957,6 @@
   </si>
   <si>
     <t>De Telegraaf</t>
-  </si>
-  <si>
-    <t>De Volkskrant</t>
   </si>
   <si>
     <t>Noordhollands Dagblad</t>
@@ -3551,11 +3548,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3893,7 +3888,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3928,15 +3923,15 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>10</v>
       </c>
       <c r="B3" t="s">
@@ -3945,7 +3940,7 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
@@ -3996,10 +3991,10 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4013,10 +4008,10 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4030,10 +4025,10 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4044,14 +4039,14 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>64</v>
+      <c r="E9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -4064,10 +4059,10 @@
       <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4084,8 +4079,8 @@
       <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>65</v>
+      <c r="E11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -4098,11 +4093,11 @@
       <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>64</v>
+      <c r="E12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -4115,11 +4110,11 @@
       <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>66</v>
+      <c r="E13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -4132,11 +4127,11 @@
       <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>67</v>
+      <c r="E14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -4149,11 +4144,11 @@
       <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>68</v>
+      <c r="E15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -4166,11 +4161,11 @@
       <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>69</v>
+      <c r="E16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -4183,10 +4178,10 @@
       <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4200,10 +4195,10 @@
       <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4217,10 +4212,10 @@
       <c r="C19" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4229,15 +4224,15 @@
         <v>69</v>
       </c>
       <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4246,15 +4241,15 @@
         <v>70</v>
       </c>
       <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4263,15 +4258,15 @@
         <v>74</v>
       </c>
       <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4280,16 +4275,16 @@
         <v>76</v>
       </c>
       <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
         <v>79</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>80</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>81</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
@@ -4297,15 +4292,15 @@
         <v>77</v>
       </c>
       <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4314,15 +4309,15 @@
         <v>86</v>
       </c>
       <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
         <v>86</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4331,15 +4326,15 @@
         <v>93</v>
       </c>
       <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" t="s">
         <v>89</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4348,15 +4343,15 @@
         <v>94</v>
       </c>
       <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
         <v>92</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4365,16 +4360,16 @@
         <v>97</v>
       </c>
       <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>68</v>
+      <c r="E28" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
@@ -4382,15 +4377,15 @@
         <v>99</v>
       </c>
       <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
         <v>98</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4399,15 +4394,15 @@
         <v>100</v>
       </c>
       <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
         <v>101</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>102</v>
       </c>
-      <c r="D30" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4416,15 +4411,15 @@
         <v>112</v>
       </c>
       <c r="B31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" t="s">
         <v>104</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4433,15 +4428,15 @@
         <v>120</v>
       </c>
       <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" t="s">
         <v>107</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4450,16 +4445,16 @@
         <v>121</v>
       </c>
       <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" t="s">
         <v>110</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>111</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>112</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
@@ -4467,16 +4462,16 @@
         <v>124</v>
       </c>
       <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" t="s">
         <v>114</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>65</v>
+      <c r="E34" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
@@ -4484,16 +4479,16 @@
         <v>126</v>
       </c>
       <c r="B35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" t="s">
         <v>117</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>118</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>113</v>
+      <c r="E35" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
@@ -4501,16 +4496,16 @@
         <v>127</v>
       </c>
       <c r="B36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" t="s">
         <v>120</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>65</v>
+      <c r="E36" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
@@ -4518,16 +4513,16 @@
         <v>128</v>
       </c>
       <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" t="s">
         <v>123</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>124</v>
       </c>
-      <c r="D37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>68</v>
+      <c r="E37" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
@@ -4535,16 +4530,16 @@
         <v>144</v>
       </c>
       <c r="B38" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" t="s">
         <v>126</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>127</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>82</v>
+      <c r="E38" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
@@ -4552,16 +4547,16 @@
         <v>146</v>
       </c>
       <c r="B39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" t="s">
         <v>129</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>69</v>
+      <c r="E39" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
@@ -4569,16 +4564,16 @@
         <v>149</v>
       </c>
       <c r="B40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" t="s">
         <v>132</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>133</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>65</v>
+      <c r="E40" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
@@ -4586,16 +4581,16 @@
         <v>152</v>
       </c>
       <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" t="s">
         <v>135</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>68</v>
+      <c r="E41" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
@@ -4603,16 +4598,16 @@
         <v>157</v>
       </c>
       <c r="B42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" t="s">
         <v>138</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>139</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>69</v>
+      <c r="E42" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
@@ -4620,15 +4615,15 @@
         <v>160</v>
       </c>
       <c r="B43" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" t="s">
         <v>141</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>142</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4637,15 +4632,15 @@
         <v>166</v>
       </c>
       <c r="B44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" t="s">
         <v>144</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4654,16 +4649,16 @@
         <v>168</v>
       </c>
       <c r="B45" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" t="s">
         <v>147</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>148</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>68</v>
+      <c r="E45" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
@@ -4671,15 +4666,15 @@
         <v>177</v>
       </c>
       <c r="B46" t="s">
+        <v>149</v>
+      </c>
+      <c r="C46" t="s">
         <v>150</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>151</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4688,15 +4683,15 @@
         <v>178</v>
       </c>
       <c r="B47" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" t="s">
         <v>153</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4705,15 +4700,15 @@
         <v>181</v>
       </c>
       <c r="B48" t="s">
+        <v>155</v>
+      </c>
+      <c r="C48" t="s">
         <v>156</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>157</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4722,15 +4717,15 @@
         <v>182</v>
       </c>
       <c r="B49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" t="s">
         <v>159</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4739,16 +4734,16 @@
         <v>200</v>
       </c>
       <c r="B50" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" t="s">
         <v>162</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>163</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>67</v>
+      <c r="E50" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
@@ -4756,16 +4751,16 @@
         <v>226</v>
       </c>
       <c r="B51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" t="s">
         <v>165</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>166</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>65</v>
+      <c r="E51" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -4773,16 +4768,16 @@
         <v>227</v>
       </c>
       <c r="B52" t="s">
+        <v>167</v>
+      </c>
+      <c r="C52" t="s">
         <v>168</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>169</v>
       </c>
-      <c r="D52" t="s">
-        <v>170</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>82</v>
+      <c r="E52" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
@@ -4790,16 +4785,16 @@
         <v>229</v>
       </c>
       <c r="B53" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" t="s">
         <v>171</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>172</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>65</v>
+      <c r="E53" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
@@ -4807,15 +4802,15 @@
         <v>230</v>
       </c>
       <c r="B54" t="s">
+        <v>173</v>
+      </c>
+      <c r="C54" t="s">
         <v>174</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4824,33 +4819,33 @@
         <v>232</v>
       </c>
       <c r="B55" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" t="s">
         <v>177</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>178</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>65</v>
+      <c r="E55" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>233</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" t="s">
         <v>180</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>181</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>65</v>
+      <c r="E56" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
@@ -4858,15 +4853,15 @@
         <v>235</v>
       </c>
       <c r="B57" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" t="s">
         <v>183</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>184</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4875,15 +4870,15 @@
         <v>236</v>
       </c>
       <c r="B58" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" t="s">
         <v>186</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4892,15 +4887,15 @@
         <v>238</v>
       </c>
       <c r="B59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D59" t="s">
         <v>189</v>
       </c>
-      <c r="C59" t="s">
-        <v>191</v>
-      </c>
-      <c r="D59" t="s">
-        <v>190</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4909,15 +4904,15 @@
         <v>239</v>
       </c>
       <c r="B60" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" t="s">
         <v>192</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>193</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4926,15 +4921,15 @@
         <v>245</v>
       </c>
       <c r="B61" t="s">
+        <v>194</v>
+      </c>
+      <c r="C61" t="s">
         <v>195</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>196</v>
       </c>
-      <c r="D61" t="s">
-        <v>197</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4943,15 +4938,15 @@
         <v>248</v>
       </c>
       <c r="B62" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" t="s">
         <v>198</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>199</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4960,15 +4955,15 @@
         <v>255</v>
       </c>
       <c r="B63" t="s">
+        <v>200</v>
+      </c>
+      <c r="C63" t="s">
         <v>201</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>202</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4977,15 +4972,15 @@
         <v>256</v>
       </c>
       <c r="B64" t="s">
+        <v>203</v>
+      </c>
+      <c r="C64" t="s">
         <v>204</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>205</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4994,15 +4989,15 @@
         <v>261</v>
       </c>
       <c r="B65" t="s">
+        <v>206</v>
+      </c>
+      <c r="C65" t="s">
         <v>207</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>208</v>
       </c>
-      <c r="D65" t="s">
-        <v>209</v>
-      </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>63</v>
       </c>
     </row>
@@ -5011,15 +5006,15 @@
         <v>262</v>
       </c>
       <c r="B66" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" t="s">
         <v>210</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>211</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" t="s">
         <v>59</v>
       </c>
     </row>
@@ -5028,15 +5023,15 @@
         <v>271</v>
       </c>
       <c r="B67" t="s">
+        <v>212</v>
+      </c>
+      <c r="C67" t="s">
         <v>213</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>214</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5045,16 +5040,16 @@
         <v>287</v>
       </c>
       <c r="B68" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" t="s">
         <v>216</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>217</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>68</v>
+      <c r="E68" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
@@ -5062,15 +5057,15 @@
         <v>296</v>
       </c>
       <c r="B69" t="s">
+        <v>218</v>
+      </c>
+      <c r="C69" t="s">
         <v>219</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>220</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5079,15 +5074,15 @@
         <v>300</v>
       </c>
       <c r="B70" t="s">
+        <v>221</v>
+      </c>
+      <c r="C70" t="s">
         <v>222</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>223</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>63</v>
       </c>
     </row>
@@ -5096,15 +5091,15 @@
         <v>306</v>
       </c>
       <c r="B71" t="s">
+        <v>224</v>
+      </c>
+      <c r="C71" t="s">
         <v>225</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>226</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>